<commit_message>
updates before first submission
</commit_message>
<xml_diff>
--- a/Tables/Formatted/Journal Pivot Percentages.xlsx
+++ b/Tables/Formatted/Journal Pivot Percentages.xlsx
@@ -2,7 +2,7 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\gorbetw\Documents\Repos\AI-Detection\Tables\Formatted\"/>
@@ -14,12 +14,12 @@
   <sheets>
     <sheet name="journal-pivot" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="20">
   <si>
     <t>Arch Pathol Lab Med</t>
   </si>
@@ -55,13 +55,37 @@
   </si>
   <si>
     <t>Greater than 50% chance of being real</t>
+  </si>
+  <si>
+    <t>AI Generated Possibility</t>
+  </si>
+  <si>
+    <t>&lt; 50%</t>
+  </si>
+  <si>
+    <t>50 - 60%</t>
+  </si>
+  <si>
+    <t>60 - 70%</t>
+  </si>
+  <si>
+    <t>70 - 80%</t>
+  </si>
+  <si>
+    <t>80 - 90%</t>
+  </si>
+  <si>
+    <t>&gt; 90%</t>
+  </si>
+  <si>
+    <t>NEJM</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="19" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <fonts count="21" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -203,6 +227,22 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="18"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="40">
     <fill>
@@ -427,7 +467,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="14">
+  <borders count="20">
     <border>
       <left/>
       <right/>
@@ -583,6 +623,74 @@
       </top>
       <bottom style="thin">
         <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
       </bottom>
       <diagonal/>
     </border>
@@ -632,7 +740,7 @@
     <xf numFmtId="0" fontId="17" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -680,6 +788,39 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="10" fontId="18" fillId="38" borderId="11" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="38" borderId="17" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="37" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="36" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="35" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="34" borderId="18" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="18" fillId="33" borderId="19" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="39" borderId="16" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="20" fillId="39" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1278,10 +1419,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H20"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="N9" sqref="N9"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A12" zoomScale="173" workbookViewId="0">
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1431,6 +1572,146 @@
       </c>
     </row>
     <row r="8" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="14" spans="2:8" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="B14" s="17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14" s="24" t="s">
+        <v>2</v>
+      </c>
+      <c r="F14" s="24" t="s">
+        <v>3</v>
+      </c>
+      <c r="G14" s="25" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B15" s="26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C15" s="18">
+        <v>0.93976805087916204</v>
+      </c>
+      <c r="D15" s="18">
+        <v>0.96687668766876689</v>
+      </c>
+      <c r="E15" s="18">
+        <v>0.95717199184228419</v>
+      </c>
+      <c r="F15" s="18">
+        <v>0.93894542090656796</v>
+      </c>
+      <c r="G15" s="18">
+        <v>0.84690553745928343</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="26" t="s">
+        <v>14</v>
+      </c>
+      <c r="C16" s="19">
+        <v>5.985783763561541E-3</v>
+      </c>
+      <c r="D16" s="19">
+        <v>3.0603060306030605E-3</v>
+      </c>
+      <c r="E16" s="19">
+        <v>7.4779061862678452E-3</v>
+      </c>
+      <c r="F16" s="19">
+        <v>6.4754856614246065E-3</v>
+      </c>
+      <c r="G16" s="19">
+        <v>8.3759888320148902E-3</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="26" t="s">
+        <v>15</v>
+      </c>
+      <c r="C17" s="20">
+        <v>7.4822297044519264E-3</v>
+      </c>
+      <c r="D17" s="20">
+        <v>3.0603060306030605E-3</v>
+      </c>
+      <c r="E17" s="20">
+        <v>5.7783820530251532E-3</v>
+      </c>
+      <c r="F17" s="20">
+        <v>5.5504162812210914E-3</v>
+      </c>
+      <c r="G17" s="20">
+        <v>1.1167985109353188E-2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="26" t="s">
+        <v>16</v>
+      </c>
+      <c r="C18" s="21">
+        <v>6.3598952487841373E-3</v>
+      </c>
+      <c r="D18" s="21">
+        <v>3.0603060306030605E-3</v>
+      </c>
+      <c r="E18" s="21">
+        <v>4.4187627464309992E-3</v>
+      </c>
+      <c r="F18" s="21">
+        <v>1.8501387604070306E-3</v>
+      </c>
+      <c r="G18" s="21">
+        <v>1.3029315960912053E-2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B19" s="26" t="s">
+        <v>17</v>
+      </c>
+      <c r="C19" s="22">
+        <v>9.3527871305649091E-3</v>
+      </c>
+      <c r="D19" s="22">
+        <v>5.0405040504050407E-3</v>
+      </c>
+      <c r="E19" s="22">
+        <v>5.7783820530251532E-3</v>
+      </c>
+      <c r="F19" s="22">
+        <v>8.3256244218316375E-3</v>
+      </c>
+      <c r="G19" s="22">
+        <v>1.8147975802698928E-2</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7" ht="30" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B20" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="C20" s="23">
+        <v>3.1051253273475497E-2</v>
+      </c>
+      <c r="D20" s="23">
+        <v>1.8901890189018902E-2</v>
+      </c>
+      <c r="E20" s="23">
+        <v>1.9374575118966689E-2</v>
+      </c>
+      <c r="F20" s="23">
+        <v>3.8852913968547641E-2</v>
+      </c>
+      <c r="G20" s="23">
+        <v>0.10237319683573755</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>